<commit_message>
LAST PHASE (AFTER LOGIN)
</commit_message>
<xml_diff>
--- a/media/Employees/Employee_Database.xlsx
+++ b/media/Employees/Employee_Database.xlsx
@@ -2745,17 +2745,17 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>MAGMA</t>
+          <t>FULLERTON</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>AUTO</t>
+          <t>RECOVERY</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">

</xml_diff>